<commit_message>
more work on poster presentation
</commit_message>
<xml_diff>
--- a/products/measurement_reports/preamplifier/measurement/measurement_preamplifier.xlsx
+++ b/products/measurement_reports/preamplifier/measurement/measurement_preamplifier.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19830" windowHeight="11790"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -428,11 +428,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="132580832"/>
-        <c:axId val="132580272"/>
+        <c:axId val="174080480"/>
+        <c:axId val="174083280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="132580832"/>
+        <c:axId val="174080480"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -551,12 +551,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="132580272"/>
+        <c:crossAx val="174083280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="132580272"/>
+        <c:axId val="174083280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="-13"/>
@@ -671,7 +671,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="132580832"/>
+        <c:crossAx val="174080480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1006,11 +1006,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="132585872"/>
-        <c:axId val="132586432"/>
+        <c:axId val="174085520"/>
+        <c:axId val="174081600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="132585872"/>
+        <c:axId val="174085520"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1129,12 +1129,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="132586432"/>
+        <c:crossAx val="174081600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="132586432"/>
+        <c:axId val="174081600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3"/>
@@ -1248,7 +1248,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="132585872"/>
+        <c:crossAx val="174085520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2763,7 +2763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added appendix and measurements preamp
</commit_message>
<xml_diff>
--- a/products/measurement_reports/preamplifier/measurement/measurement_preamplifier.xlsx
+++ b/products/measurement_reports/preamplifier/measurement/measurement_preamplifier.xlsx
@@ -428,11 +428,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="174080480"/>
-        <c:axId val="174083280"/>
+        <c:axId val="133834000"/>
+        <c:axId val="133834560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="174080480"/>
+        <c:axId val="133834000"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -551,12 +551,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174083280"/>
+        <c:crossAx val="133834560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="174083280"/>
+        <c:axId val="133834560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="-13"/>
@@ -671,7 +671,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174080480"/>
+        <c:crossAx val="133834000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1006,11 +1006,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="174085520"/>
-        <c:axId val="174081600"/>
+        <c:axId val="133836800"/>
+        <c:axId val="133837360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="174085520"/>
+        <c:axId val="133836800"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1129,12 +1129,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174081600"/>
+        <c:crossAx val="133837360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="174081600"/>
+        <c:axId val="133837360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3"/>
@@ -1248,7 +1248,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174085520"/>
+        <c:crossAx val="133836800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2763,8 +2763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" topLeftCell="F33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>